<commit_message>
Several updates and initial results
</commit_message>
<xml_diff>
--- a/RedLightAreas/Population_distribution.xlsx
+++ b/RedLightAreas/Population_distribution.xlsx
@@ -14,30 +14,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Delhi</t>
+    <t>RLAC1</t>
   </si>
   <si>
-    <t>Delhi_RL</t>
+    <t>RLA1</t>
   </si>
   <si>
-    <t>Kolkata</t>
+    <t>RLAC2</t>
   </si>
   <si>
-    <t>Kolkata_RL</t>
+    <t>RLA2</t>
   </si>
   <si>
-    <t>Mumbai</t>
+    <t>RLAC3</t>
   </si>
   <si>
-    <t>Mumbai_RL</t>
+    <t>RLA3</t>
   </si>
   <si>
-    <t>Nagpur</t>
+    <t>RLAC4</t>
   </si>
   <si>
-    <t>Nagpur_RL</t>
+    <t>RLA4</t>
+  </si>
+  <si>
+    <t>RLAC5</t>
+  </si>
+  <si>
+    <t>RLA5</t>
   </si>
 </sst>
 </file>
@@ -395,13 +401,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,614 +432,746 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>899977.292268031</v>
+        <v>1908625.34286768</v>
       </c>
       <c r="C2">
-        <v>82.3552750038325</v>
+        <v>511.628665962775</v>
       </c>
       <c r="D2">
-        <v>372546.015976892</v>
+        <v>270523.399976297</v>
       </c>
       <c r="E2">
-        <v>80.4393184547738</v>
+        <v>216.007277547613</v>
       </c>
       <c r="F2">
-        <v>1061220.57251515</v>
+        <v>1823438.05722011</v>
       </c>
       <c r="G2">
-        <v>83.6144252506217</v>
+        <v>378.527038750103</v>
       </c>
       <c r="H2">
-        <v>186294.44451804</v>
+        <v>1388618.21280609</v>
       </c>
       <c r="I2">
-        <v>83.6144252506217</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>1496.15430336009</v>
+      </c>
+      <c r="J2">
+        <v>619875.429810878</v>
+      </c>
+      <c r="K2">
+        <v>593.318690926236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1000825.31245259</v>
+        <v>2147550.37154152</v>
       </c>
       <c r="C3">
-        <v>91.5836927730861</v>
+        <v>575.675229182905</v>
       </c>
       <c r="D3">
-        <v>419013.836698446</v>
+        <v>304387.988088267</v>
       </c>
       <c r="E3">
-        <v>90.4725483609347</v>
+        <v>243.047442960213</v>
       </c>
       <c r="F3">
-        <v>1113207.76724538</v>
+        <v>2051699.19381998</v>
       </c>
       <c r="G3">
-        <v>87.7105382740039</v>
+        <v>425.911709568373</v>
       </c>
       <c r="H3">
-        <v>195420.65806417</v>
+        <v>1562447.84760137</v>
       </c>
       <c r="I3">
-        <v>87.7105382740039</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>1683.44549236511</v>
+      </c>
+      <c r="J3">
+        <v>697472.510555521</v>
+      </c>
+      <c r="K3">
+        <v>667.59135306604</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1073917.51688364</v>
+        <v>2245362.99809218</v>
       </c>
       <c r="C4">
-        <v>98.2722266375192</v>
+        <v>601.895012873527</v>
       </c>
       <c r="D4">
-        <v>465179.277678177</v>
+        <v>318251.685536264</v>
       </c>
       <c r="E4">
-        <v>100.440489096621</v>
+        <v>254.117315447207</v>
       </c>
       <c r="F4">
-        <v>1216799.58786527</v>
+        <v>2145146.16935954</v>
       </c>
       <c r="G4">
-        <v>95.872621413109</v>
+        <v>445.310343259867</v>
       </c>
       <c r="H4">
-        <v>213605.926215592</v>
+        <v>1633611.31358919</v>
       </c>
       <c r="I4">
-        <v>95.872621413109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>1760.11993383347</v>
+      </c>
+      <c r="J4">
+        <v>729239.690086379</v>
+      </c>
+      <c r="K4">
+        <v>697.997561260835</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1086446.3058901</v>
+        <v>2039237.7047348</v>
       </c>
       <c r="C5">
-        <v>99.4187131910767</v>
+        <v>546.640790636716</v>
       </c>
       <c r="D5">
-        <v>460175.583872452</v>
+        <v>289036.043300073</v>
       </c>
       <c r="E5">
-        <v>99.3601025075078</v>
+        <v>230.789236095115</v>
       </c>
       <c r="F5">
-        <v>1204640.35989767</v>
+        <v>1948220.82417954</v>
       </c>
       <c r="G5">
-        <v>94.9145860297653</v>
+        <v>404.43066134763</v>
       </c>
       <c r="H5">
-        <v>211471.406136866</v>
+        <v>1483645.08918288</v>
       </c>
       <c r="I5">
-        <v>94.9145860297653</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>1598.54016342937</v>
+      </c>
+      <c r="J5">
+        <v>662295.171460831</v>
+      </c>
+      <c r="K5">
+        <v>633.921083559959</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1149445.36793972</v>
+        <v>1885233.29616341</v>
       </c>
       <c r="C6">
-        <v>105.183642067232</v>
+        <v>505.358162590196</v>
       </c>
       <c r="D6">
-        <v>444949.453153002</v>
+        <v>267207.874469685</v>
       </c>
       <c r="E6">
-        <v>96.0725097666105</v>
+        <v>213.359899766669</v>
       </c>
       <c r="F6">
-        <v>1257202.37139547</v>
+        <v>1801090.06296539</v>
       </c>
       <c r="G6">
-        <v>99.0559893301073</v>
+        <v>373.88782435302</v>
       </c>
       <c r="H6">
-        <v>220698.527235287</v>
+        <v>1371599.35564287</v>
       </c>
       <c r="I6">
-        <v>99.0559893301073</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>1477.81748756134</v>
+      </c>
+      <c r="J6">
+        <v>612278.257815259</v>
+      </c>
+      <c r="K6">
+        <v>586.046997411045</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1087065.96879551</v>
+        <v>1715865.5459488</v>
       </c>
       <c r="C7">
-        <v>99.4754174095307</v>
+        <v>459.957216604002</v>
       </c>
       <c r="D7">
-        <v>406318.154997895</v>
+        <v>243202.147098618</v>
       </c>
       <c r="E7">
-        <v>87.7313246207393</v>
+        <v>194.191828481786</v>
       </c>
       <c r="F7">
-        <v>1150213.11276383</v>
+        <v>1639281.66900209</v>
       </c>
       <c r="G7">
-        <v>90.6262193085249</v>
+        <v>340.298061339511</v>
       </c>
       <c r="H7">
-        <v>201916.847891341</v>
+        <v>1248376.04024005</v>
       </c>
       <c r="I7">
-        <v>90.6262193085249</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>1345.05162584787</v>
+      </c>
+      <c r="J7">
+        <v>557271.701734096</v>
+      </c>
+      <c r="K7">
+        <v>533.397035375296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>934836.751549125</v>
+        <v>1498975.25420609</v>
       </c>
       <c r="C8">
-        <v>85.5452003277754</v>
+        <v>401.817314480584</v>
       </c>
       <c r="D8">
-        <v>347573.625312822</v>
+        <v>212460.703072766</v>
       </c>
       <c r="E8">
-        <v>75.0473346485942</v>
+        <v>169.645428309052</v>
       </c>
       <c r="F8">
-        <v>997094.21342763</v>
+        <v>1432071.79741408</v>
       </c>
       <c r="G8">
-        <v>78.561857671942</v>
+        <v>297.283417227292</v>
       </c>
       <c r="H8">
-        <v>175037.233006525</v>
+        <v>1090577.75341534</v>
       </c>
       <c r="I8">
-        <v>78.561857671942</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>1175.03326967309</v>
+      </c>
+      <c r="J8">
+        <v>486830.971541432</v>
+      </c>
+      <c r="K8">
+        <v>465.974131004735</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>859607.329105739</v>
+        <v>1440531.05737572</v>
       </c>
       <c r="C9">
-        <v>78.6610935542687</v>
+        <v>386.150684793765</v>
       </c>
       <c r="D9">
-        <v>356263.791495173</v>
+        <v>204176.980500121</v>
       </c>
       <c r="E9">
-        <v>76.9236962656525</v>
+        <v>163.031049068538</v>
       </c>
       <c r="F9">
-        <v>934846.352362624</v>
+        <v>1376236.12850064</v>
       </c>
       <c r="G9">
-        <v>73.6572984682928</v>
+        <v>285.69250503439</v>
       </c>
       <c r="H9">
-        <v>164109.786818729</v>
+        <v>1048056.74401203</v>
       </c>
       <c r="I9">
-        <v>73.6572984682928</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>1129.21938748771</v>
+      </c>
+      <c r="J9">
+        <v>467849.7074785</v>
+      </c>
+      <c r="K9">
+        <v>447.806063350594</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>714923.533988276</v>
+        <v>1225610.89682649</v>
       </c>
       <c r="C10">
-        <v>65.4213442429626</v>
+        <v>328.538898677011</v>
       </c>
       <c r="D10">
-        <v>312594.202658638</v>
+        <v>173714.777547354</v>
       </c>
       <c r="E10">
-        <v>67.4946544491674</v>
+        <v>138.70761705302</v>
       </c>
       <c r="F10">
-        <v>815703.533449915</v>
+        <v>1170908.45564238</v>
       </c>
       <c r="G10">
-        <v>64.2699396249617</v>
+        <v>243.068586073864</v>
       </c>
       <c r="H10">
-        <v>143194.582343328</v>
+        <v>891691.823912274</v>
       </c>
       <c r="I10">
-        <v>64.2699396249617</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>960.74539950144</v>
+      </c>
+      <c r="J10">
+        <v>398048.828330941</v>
+      </c>
+      <c r="K10">
+        <v>380.99559748979</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>593738.059961938</v>
+        <v>1054389.99629362</v>
       </c>
       <c r="C11">
-        <v>54.3318832913895</v>
+        <v>282.641194734256</v>
       </c>
       <c r="D11">
-        <v>271070.788585768</v>
+        <v>149446.389656432</v>
       </c>
       <c r="E11">
-        <v>58.5290099792391</v>
+        <v>119.329816835934</v>
       </c>
       <c r="F11">
-        <v>683801.16521267</v>
+        <v>1007329.622641</v>
       </c>
       <c r="G11">
-        <v>53.8772455941496</v>
+        <v>209.111298074399</v>
       </c>
       <c r="H11">
-        <v>120039.472974186</v>
+        <v>767120.25108815</v>
       </c>
       <c r="I11">
-        <v>53.8772455941496</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>826.526869859286</v>
+      </c>
+      <c r="J11">
+        <v>342440.413768575</v>
+      </c>
+      <c r="K11">
+        <v>327.769561828573</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>447948.515159435</v>
+        <v>830223.355373301</v>
       </c>
       <c r="C12">
-        <v>40.9909488499925</v>
+        <v>222.550784703811</v>
       </c>
       <c r="D12">
-        <v>216313.282109416</v>
+        <v>117673.615555091</v>
       </c>
       <c r="E12">
-        <v>46.7058893113379</v>
+        <v>93.959921165662</v>
       </c>
       <c r="F12">
-        <v>557622.933660247</v>
+        <v>793168.165684159</v>
       </c>
       <c r="G12">
-        <v>43.9355609117741</v>
+        <v>164.653576137922</v>
       </c>
       <c r="H12">
-        <v>97889.2205515291</v>
+        <v>604028.064636398</v>
       </c>
       <c r="I12">
-        <v>43.9355609117741</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>650.80464876649</v>
+      </c>
+      <c r="J12">
+        <v>269636.501042066</v>
+      </c>
+      <c r="K12">
+        <v>258.084718526461</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>331589.374614004</v>
+        <v>662328.576092227</v>
       </c>
       <c r="C13">
-        <v>30.3431368427819</v>
+        <v>177.544685279066</v>
       </c>
       <c r="D13">
-        <v>166057.382915193</v>
+        <v>93876.6631049342</v>
       </c>
       <c r="E13">
-        <v>35.854745811884</v>
+        <v>74.958552289111</v>
       </c>
       <c r="F13">
-        <v>440471.51308567</v>
+        <v>632766.999843145</v>
       </c>
       <c r="G13">
-        <v>34.7051059504449</v>
+        <v>131.35593924949</v>
       </c>
       <c r="H13">
-        <v>77323.6007494983</v>
+        <v>481876.407572856</v>
       </c>
       <c r="I13">
-        <v>34.7051059504449</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>519.193435768734</v>
+      </c>
+      <c r="J13">
+        <v>215108.330356934</v>
+      </c>
+      <c r="K13">
+        <v>205.892646872039</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>307563.264928369</v>
+        <v>637248.106550324</v>
       </c>
       <c r="C14">
-        <v>28.1445515146496</v>
+        <v>170.821581019031</v>
       </c>
       <c r="D14">
-        <v>139477.431402582</v>
+        <v>90321.8251065644</v>
       </c>
       <c r="E14">
-        <v>30.1156609940557</v>
+        <v>72.1200884881313</v>
       </c>
       <c r="F14">
-        <v>412888.69641838</v>
+        <v>608805.941782927</v>
       </c>
       <c r="G14">
-        <v>32.5318335675296</v>
+        <v>126.38186935063</v>
       </c>
       <c r="H14">
-        <v>72481.5107614601</v>
+        <v>463629.140280844</v>
       </c>
       <c r="I14">
-        <v>32.5318335675296</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>499.533080437273</v>
+      </c>
+      <c r="J14">
+        <v>206962.799388668</v>
+      </c>
+      <c r="K14">
+        <v>198.096087210906</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>177527.232285701</v>
+        <v>447602.98888187</v>
       </c>
       <c r="C15">
-        <v>16.2451921411412</v>
+        <v>119.985056752156</v>
       </c>
       <c r="D15">
-        <v>100742.088605127</v>
+        <v>63442.0384515825</v>
       </c>
       <c r="E15">
-        <v>21.7520107572684</v>
+        <v>50.6571409689442</v>
       </c>
       <c r="F15">
-        <v>348942.68311615</v>
+        <v>427625.215971607</v>
       </c>
       <c r="G15">
-        <v>27.4934755788012</v>
+        <v>88.7706089360545</v>
       </c>
       <c r="H15">
-        <v>61255.9584721295</v>
+        <v>325653.04908607</v>
       </c>
       <c r="I15">
-        <v>27.4934755788012</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>350.871972079267</v>
+      </c>
+      <c r="J15">
+        <v>145370.643932091</v>
+      </c>
+      <c r="K15">
+        <v>139.142666427684</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>123313.56976667</v>
+        <v>325002.480332707</v>
       </c>
       <c r="C16">
-        <v>11.28419909823</v>
+        <v>87.120600210297</v>
       </c>
       <c r="D16">
-        <v>70647.0741999137</v>
+        <v>46064.9735731969</v>
       </c>
       <c r="E16">
-        <v>15.2539612712363</v>
+        <v>36.7819180622484</v>
       </c>
       <c r="F16">
-        <v>242932.460655186</v>
+        <v>310496.710915084</v>
       </c>
       <c r="G16">
-        <v>19.1408446071306</v>
+        <v>64.4559326043211</v>
       </c>
       <c r="H16">
-        <v>42646.1463198899</v>
+        <v>236455.187543026</v>
       </c>
       <c r="I16">
-        <v>19.1408446071306</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>254.76653203289</v>
+      </c>
+      <c r="J16">
+        <v>105552.958802877</v>
+      </c>
+      <c r="K16">
+        <v>101.030852859293</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>65610.6382061576</v>
+        <v>156208.603031831</v>
       </c>
       <c r="C17">
-        <v>6.00390943090132</v>
+        <v>41.8734873660457</v>
       </c>
       <c r="D17">
-        <v>37582.418425657</v>
+        <v>22140.5853986128</v>
       </c>
       <c r="E17">
-        <v>8.11471333578694</v>
+        <v>17.6787944247479</v>
       </c>
       <c r="F17">
-        <v>120469.284267491</v>
+        <v>149236.576312807</v>
       </c>
       <c r="G17">
-        <v>9.49187211901345</v>
+        <v>30.9799826109868</v>
       </c>
       <c r="H17">
-        <v>21148.0619348601</v>
+        <v>113649.392730522</v>
       </c>
       <c r="I17">
-        <v>9.49187211901345</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>122.450524154098</v>
+      </c>
+      <c r="J17">
+        <v>50732.7827885947</v>
+      </c>
+      <c r="K17">
+        <v>48.5592859848594</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>41068.4685614462</v>
+        <v>105242.671746555</v>
       </c>
       <c r="C18">
-        <v>3.75810040033417</v>
+        <v>28.2114915581843</v>
       </c>
       <c r="D18">
-        <v>22648.1512170902</v>
+        <v>14916.8119819109</v>
       </c>
       <c r="E18">
-        <v>4.89013912385092</v>
+        <v>11.9107624190163</v>
       </c>
       <c r="F18">
-        <v>72166.7659022035</v>
+        <v>100545.397043644</v>
       </c>
       <c r="G18">
-        <v>5.68607771974075</v>
+        <v>20.872193191419</v>
       </c>
       <c r="H18">
-        <v>12668.6835089813</v>
+        <v>76569.1869793904</v>
       </c>
       <c r="I18">
-        <v>5.68607771974075</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>82.4987873178617</v>
+      </c>
+      <c r="J18">
+        <v>34180.2788206316</v>
+      </c>
+      <c r="K18">
+        <v>32.7159253457395</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>16951.1361557724</v>
+        <v>40321.8052419327</v>
       </c>
       <c r="C19">
-        <v>1.5511674480341</v>
+        <v>10.8087171231547</v>
       </c>
       <c r="D19">
-        <v>10010.4865973794</v>
+        <v>5715.10374625992</v>
       </c>
       <c r="E19">
-        <v>2.16144230446903</v>
+        <v>4.56339082400982</v>
       </c>
       <c r="F19">
-        <v>28043.0328132835</v>
+        <v>38522.1303325504</v>
       </c>
       <c r="G19">
-        <v>2.20953318442529</v>
+        <v>7.99679915826483</v>
       </c>
       <c r="H19">
-        <v>4922.87970649686</v>
+        <v>29336.0838686346</v>
       </c>
       <c r="I19">
-        <v>2.20953318442529</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>31.6079018113234</v>
+      </c>
+      <c r="J19">
+        <v>13095.5488192039</v>
+      </c>
+      <c r="K19">
+        <v>12.5345085620529</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>8973.70928838352</v>
+        <v>24474.5174063898</v>
       </c>
       <c r="C20">
-        <v>0.821167714561816</v>
+        <v>6.56067191893201</v>
       </c>
       <c r="D20">
-        <v>6302.72774363259</v>
+        <v>3468.95197965243</v>
       </c>
       <c r="E20">
-        <v>1.36087114708334</v>
+        <v>2.76988561112932</v>
       </c>
       <c r="F20">
-        <v>17896.9671000836</v>
+        <v>23382.1512627799</v>
       </c>
       <c r="G20">
-        <v>1.41011647960812</v>
+        <v>4.85389478521709</v>
       </c>
       <c r="H20">
-        <v>3141.76489866352</v>
+        <v>17806.407500117</v>
       </c>
       <c r="I20">
-        <v>1.41011647960812</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>19.185354882281</v>
+      </c>
+      <c r="J20">
+        <v>7948.73234466504</v>
+      </c>
+      <c r="K20">
+        <v>7.60819229550455</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>4090.68740288061</v>
+        <v>10715.0184163763</v>
       </c>
       <c r="C21">
-        <v>0.374331318037982</v>
+        <v>2.8722821891804</v>
       </c>
       <c r="D21">
-        <v>2919.39715455052</v>
+        <v>1518.71776388107</v>
       </c>
       <c r="E21">
-        <v>0.630349828852864</v>
+        <v>1.21266437420162</v>
       </c>
       <c r="F21">
-        <v>9103.77816088198</v>
+        <v>10236.7771848188</v>
       </c>
       <c r="G21">
-        <v>0.717294027505711</v>
+        <v>2.12504995098188</v>
       </c>
       <c r="H21">
-        <v>1598.14400457522</v>
+        <v>7795.69954843897</v>
       </c>
       <c r="I21">
-        <v>0.717294027505711</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>8.399406920877</v>
+      </c>
+      <c r="J21">
+        <v>3479.97927990585</v>
+      </c>
+      <c r="K21">
+        <v>3.33088980706029</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>2565.96479651861</v>
+        <v>10249.4128761633</v>
       </c>
       <c r="C22">
-        <v>0.234806742662245</v>
+        <v>2.74747134440448</v>
       </c>
       <c r="D22">
-        <v>3006.82920019538</v>
+        <v>1452.72409243743</v>
       </c>
       <c r="E22">
-        <v>0.649227964334562</v>
+        <v>1.15996980764966</v>
       </c>
       <c r="F22">
-        <v>6568.84868480956</v>
+        <v>9791.95292171792</v>
       </c>
       <c r="G22">
-        <v>0.517564888548006</v>
+        <v>2.03270899626226</v>
       </c>
       <c r="H22">
-        <v>1153.14388785295</v>
+        <v>7456.94876346211</v>
       </c>
       <c r="I22">
-        <v>0.517564888548006</v>
+        <v>8.03442291012752</v>
+      </c>
+      <c r="J22">
+        <v>3328.76184195221</v>
+      </c>
+      <c r="K22">
+        <v>3.18615083529745</v>
       </c>
     </row>
   </sheetData>

</xml_diff>